<commit_message>
Auth Guards and Displaying Usernames
</commit_message>
<xml_diff>
--- a/loginpage/src/backend/Users.xlsx
+++ b/loginpage/src/backend/Users.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruthi.abbaraju\Desktop\zforms\Angular\loginpage\src\app\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruthi.abbaraju\Desktop\zforms\Angular\loginpage\src\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358BFE4A-59FC-4535-BB6E-A39B4F746CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0222215-0D5C-47D2-808E-990A8535467A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Role</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>abc.123@gmail.com</t>
   </si>
@@ -52,6 +43,30 @@
   </si>
   <si>
     <t>def456</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin@gmail.com</t>
+  </si>
+  <si>
+    <t>DEF</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>username</t>
   </si>
 </sst>
 </file>
@@ -391,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -403,54 +418,67 @@
     <col min="2" max="2" width="20.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{C67CD05E-C09F-427A-BFAA-186572E26065}"/>
     <hyperlink ref="A4" r:id="rId2" xr:uid="{84D809C0-18C0-4085-B52F-87072BA3745E}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{0764FC00-B02A-4C56-874B-F538C0699B9F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>